<commit_message>
réajustement de Gantt car associé part en vacances
</commit_message>
<xml_diff>
--- a/organisation personnelle/gantt.xlsx
+++ b/organisation personnelle/gantt.xlsx
@@ -598,7 +598,7 @@
   <dimension ref="B1:Z45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -663,11 +663,11 @@
       </c>
       <c r="D7" s="4" t="n">
         <f aca="false">SUM(D10:D35)</f>
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E7" s="5" t="n">
         <f aca="false">SUM(E10:E35)</f>
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F7" s="5" t="n">
         <f aca="false">SUM(F10:F35)</f>
@@ -992,10 +992,10 @@
       </c>
       <c r="C13" s="19" t="n">
         <f aca="false">SUM(D13:Z13)</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D13" s="20" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
@@ -1026,11 +1026,11 @@
       </c>
       <c r="C14" s="19" t="n">
         <f aca="false">SUM(D14:Z14)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
@@ -2068,7 +2068,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{50BDA8B3-3EF0-42D4-8D1B-D5355790F3E2}</x14:id>
+          <x14:id>{904AA076-2044-406D-98BC-335062F7AA43}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2112,7 +2112,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{59D6B3B2-2E62-4A86-BB19-3D7B965B8C86}</x14:id>
+          <x14:id>{8010B188-9A5F-4280-89CB-5B77EB972167}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2126,7 +2126,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B155CEB2-E0D4-47B6-86C2-445DE174E08B}</x14:id>
+          <x14:id>{B6826BBD-722B-4754-AC71-60EB90B17670}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2170,7 +2170,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E5EC5FB5-1A4E-4168-858A-D58A4B9079AA}</x14:id>
+          <x14:id>{801A6069-8D4F-49F1-826C-FB98819ADED6}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2214,7 +2214,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D8FCFACD-9D35-40C5-A27D-A96E77194F80}</x14:id>
+          <x14:id>{B961DD3A-C631-4430-B8E9-7D4750DBC0D9}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2258,7 +2258,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6668F520-F7F1-4073-B7B3-B011F8491FA3}</x14:id>
+          <x14:id>{E8843F1A-A7DE-44D7-A44B-76371D134D89}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2302,7 +2302,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D09EC41B-23B0-44C5-9986-ADB393C41F21}</x14:id>
+          <x14:id>{E5E19293-30F7-445B-9E1A-C3D0936ABEDF}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -2418,7 +2418,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{50BDA8B3-3EF0-42D4-8D1B-D5355790F3E2}">
+          <x14:cfRule type="dataBar" id="{904AA076-2044-406D-98BC-335062F7AA43}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2429,7 +2429,7 @@
           <xm:sqref>C10:C28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{59D6B3B2-2E62-4A86-BB19-3D7B965B8C86}">
+          <x14:cfRule type="dataBar" id="{8010B188-9A5F-4280-89CB-5B77EB972167}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="true">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2440,7 +2440,7 @@
           <xm:sqref>C9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B155CEB2-E0D4-47B6-86C2-445DE174E08B}">
+          <x14:cfRule type="dataBar" id="{B6826BBD-722B-4754-AC71-60EB90B17670}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2451,7 +2451,7 @@
           <xm:sqref>C29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E5EC5FB5-1A4E-4168-858A-D58A4B9079AA}">
+          <x14:cfRule type="dataBar" id="{801A6069-8D4F-49F1-826C-FB98819ADED6}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2462,7 +2462,7 @@
           <xm:sqref>C30:C34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D8FCFACD-9D35-40C5-A27D-A96E77194F80}">
+          <x14:cfRule type="dataBar" id="{B961DD3A-C631-4430-B8E9-7D4750DBC0D9}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2473,7 +2473,7 @@
           <xm:sqref>C35:C39</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6668F520-F7F1-4073-B7B3-B011F8491FA3}">
+          <x14:cfRule type="dataBar" id="{E8843F1A-A7DE-44D7-A44B-76371D134D89}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -2484,7 +2484,7 @@
           <xm:sqref>C40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D09EC41B-23B0-44C5-9986-ADB393C41F21}">
+          <x14:cfRule type="dataBar" id="{E5E19293-30F7-445B-9E1A-C3D0936ABEDF}">
             <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>

</xml_diff>